<commit_message>
HL-319: apprenticeship benefit calculation, TrainingCompensation model and API
</commit_message>
<xml_diff>
--- a/backend/benefit/calculator/tests/Helsinki-lisä laskurin testitapaukset.xlsx
+++ b/backend/benefit/calculator/tests/Helsinki-lisä laskurin testitapaukset.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\KANSLIAS000002\HOME2$\VUORESO\System\Desktop\Digitalisointi\LAsketa esimerkit\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1155" documentId="8_{EAB5B95F-C968-4491-B346-1A0F472715C5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{84FC86AD-72E8-4E3D-BD03-D694D12502B8}"/>
+  <xr:revisionPtr revIDLastSave="1333" documentId="8_{EAB5B95F-C968-4491-B346-1A0F472715C5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9662124A-12C0-4C52-9FC5-BB92E6D53103}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12432" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12432" firstSheet="2" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Palkan Helsinki-lisä" sheetId="5" r:id="rId1"/>
@@ -237,7 +237,7 @@
     <author>tc={6EF342C0-8BFF-45D2-8DB7-F300C749412C}</author>
   </authors>
   <commentList>
-    <comment ref="C41" authorId="0" shapeId="0" xr:uid="{E9CF2E1B-48CE-478B-9C46-178E6E0F38C0}">
+    <comment ref="C51" authorId="0" shapeId="0" xr:uid="{E9CF2E1B-48CE-478B-9C46-178E6E0F38C0}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -245,7 +245,7 @@
     Lasketaan esim. (0,3x(1752+469))+((1106/12)x0,3)=691,25</t>
       </text>
     </comment>
-    <comment ref="B42" authorId="1" shapeId="0" xr:uid="{6EF342C0-8BFF-45D2-8DB7-F300C749412C}">
+    <comment ref="B52" authorId="1" shapeId="0" xr:uid="{6EF342C0-8BFF-45D2-8DB7-F300C749412C}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -258,7 +258,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="303" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="319" uniqueCount="112">
   <si>
     <t>Ensimmäisessä sarakkeessa testin ajoon liittyvät ohjauskoodit</t>
   </si>
@@ -521,19 +521,79 @@
     <t>expected_results.total_amount</t>
   </si>
   <si>
+    <t>oy</t>
+  </si>
+  <si>
     <t>Palkkatuettu oppisopimus</t>
   </si>
   <si>
-    <t>1.9.2021</t>
-  </si>
-  <si>
-    <t>31.10.2021</t>
+    <t xml:space="preserve"> </t>
   </si>
   <si>
     <t>Palkkatukipäätöksen tiedot (jätä tyhjäksi jos päätöstä ei ole)</t>
   </si>
   <si>
-    <t>Koulutustuki eur/kk</t>
+    <t>Koulutuskorvauksen tiedot (jätä tyhjäksi jos koulutuskorvausta ei ole)</t>
+  </si>
+  <si>
+    <t>application.training_compensation_1.monthly_amount</t>
+  </si>
+  <si>
+    <t>Koulutuskorvaus eur/kk</t>
+  </si>
+  <si>
+    <t>application.training_compensation_1.start_date</t>
+  </si>
+  <si>
+    <t>Koulutuskorvauksen alkupäivä</t>
+  </si>
+  <si>
+    <t>application.training_compensation_1.end_date</t>
+  </si>
+  <si>
+    <t>Koulutuskorvauksen päättymispäivä</t>
+  </si>
+  <si>
+    <t>Toisen koulutuskorvauksen tiedot (jätä tyhjäksi jos sama koulutuskorvaus koko hakuajan)</t>
+  </si>
+  <si>
+    <t>application.training_compensation_2.monthly_amount</t>
+  </si>
+  <si>
+    <t>application.training_compensation_2.start_date</t>
+  </si>
+  <si>
+    <t>application.training_compensation_2.end_date</t>
+  </si>
+  <si>
+    <t>expected_results.time_range_1.training_compensation_monthly_eur</t>
+  </si>
+  <si>
+    <t>expected_results.time_range_2.training_compensation_monthly_eur</t>
+  </si>
+  <si>
+    <t>Ajanjakso #3 (jätä tyhjäksi jos koko jakso lasketaan samoilla perusteilla)</t>
+  </si>
+  <si>
+    <t>expected_results.time_range_3.pay_subsidy_monthly_eur</t>
+  </si>
+  <si>
+    <t>expected_results.time_range_3.training_compensation_monthly_eur</t>
+  </si>
+  <si>
+    <t>expected_results.time_range_3.start_date</t>
+  </si>
+  <si>
+    <t>expected_results.time_range_3.end_date</t>
+  </si>
+  <si>
+    <t>expected_results.time_range_3.duration</t>
+  </si>
+  <si>
+    <t>expected_results.time_range_3.monthly_amount</t>
+  </si>
+  <si>
+    <t>expected_results.time_range_3.total_amount</t>
   </si>
 </sst>
 </file>
@@ -603,7 +663,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
@@ -628,6 +688,10 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="14" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="166" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1024,10 +1088,10 @@
 
 <file path=xl/threadedComments/threadedComment3.xml><?xml version="1.0" encoding="utf-8"?>
 <ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <threadedComment ref="C41" dT="2021-09-21T08:21:03.20" personId="{6D75A251-2E9C-408D-92F0-CE49CCF1513F}" id="{E9CF2E1B-48CE-478B-9C46-178E6E0F38C0}">
+  <threadedComment ref="C51" dT="2021-09-21T08:21:03.20" personId="{6D75A251-2E9C-408D-92F0-CE49CCF1513F}" id="{E9CF2E1B-48CE-478B-9C46-178E6E0F38C0}">
     <text>Lasketaan esim. (0,3x(1752+469))+((1106/12)x0,3)=691,25</text>
   </threadedComment>
-  <threadedComment ref="B42" dT="2021-09-21T08:15:13.41" personId="{6D75A251-2E9C-408D-92F0-CE49CCF1513F}" id="{6EF342C0-8BFF-45D2-8DB7-F300C749412C}">
+  <threadedComment ref="B52" dT="2021-09-21T08:15:13.41" personId="{6D75A251-2E9C-408D-92F0-CE49CCF1513F}" id="{6EF342C0-8BFF-45D2-8DB7-F300C749412C}">
     <text>Koulutuskorvaus</text>
   </threadedComment>
 </ThreadedComments>
@@ -1037,8 +1101,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C618BC34-3A38-45D6-9211-F1F705D1E76B}">
   <dimension ref="A1:AV67"/>
   <sheetViews>
-    <sheetView topLeftCell="D39" workbookViewId="0">
-      <selection activeCell="O49" sqref="O49"/>
+    <sheetView topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="D1" sqref="D1:D1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75"/>
@@ -2806,7 +2870,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A670E8AE-FBF8-4578-9728-3F8C1DE2072A}">
   <dimension ref="A5:O44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A20" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A26" sqref="A26"/>
     </sheetView>
   </sheetViews>
@@ -3467,10 +3531,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1B14CE17-365F-4CD6-A28B-9E2140F5A365}">
-  <dimension ref="A5:T55"/>
+  <dimension ref="A5:S89"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="C30" sqref="C30"/>
+    <sheetView tabSelected="1" topLeftCell="A38" workbookViewId="0">
+      <selection activeCell="B43" sqref="B43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75"/>
@@ -3482,7 +3546,7 @@
     <col min="10" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
-    <row r="5" spans="1:20">
+    <row r="5" spans="1:14">
       <c r="B5" s="5" t="s">
         <v>1</v>
       </c>
@@ -3490,15 +3554,15 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:20">
+    <row r="7" spans="1:14">
       <c r="B7" s="5" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:20">
+    <row r="8" spans="1:14">
       <c r="B8" s="5"/>
     </row>
-    <row r="9" spans="1:20">
+    <row r="9" spans="1:14">
       <c r="A9" s="1" t="s">
         <v>6</v>
       </c>
@@ -3506,7 +3570,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:20">
+    <row r="10" spans="1:14">
       <c r="A10" s="1" t="s">
         <v>9</v>
       </c>
@@ -3516,8 +3580,8 @@
       <c r="C10" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="D10" s="1" t="s">
-        <v>11</v>
+      <c r="D10" s="15" t="s">
+        <v>87</v>
       </c>
       <c r="E10" s="1" t="s">
         <v>11</v>
@@ -3525,50 +3589,8 @@
       <c r="F10" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="G10" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="H10" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="I10" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="J10" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="K10" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="L10" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="M10" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="N10" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="O10" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="P10" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="Q10" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="R10" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="S10" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="T10" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="11" spans="1:20">
+    </row>
+    <row r="11" spans="1:14">
       <c r="A11" s="1" t="s">
         <v>12</v>
       </c>
@@ -3588,7 +3610,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="12" spans="1:20">
+    <row r="12" spans="1:14">
       <c r="A12" s="1" t="s">
         <v>16</v>
       </c>
@@ -3596,28 +3618,19 @@
         <v>17</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="G12" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="H12" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="I12" s="1" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="13" spans="1:20">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14">
       <c r="A13" s="1" t="s">
         <v>19</v>
       </c>
@@ -3633,35 +3646,19 @@
       <c r="E13" s="4">
         <v>44235</v>
       </c>
-      <c r="F13" s="4" t="s">
-        <v>88</v>
-      </c>
-      <c r="G13" s="4" t="s">
-        <v>88</v>
-      </c>
-      <c r="H13" s="4" t="s">
-        <v>88</v>
-      </c>
-      <c r="I13" s="4" t="s">
-        <v>88</v>
-      </c>
-      <c r="J13" s="4" t="s">
-        <v>88</v>
-      </c>
-      <c r="K13" s="4" t="s">
-        <v>88</v>
-      </c>
-      <c r="L13" s="4" t="s">
-        <v>88</v>
-      </c>
-      <c r="M13" s="4" t="s">
-        <v>88</v>
-      </c>
-      <c r="N13" s="4" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="14" spans="1:20">
+      <c r="F13" s="4">
+        <v>44411</v>
+      </c>
+      <c r="G13" s="4"/>
+      <c r="H13" s="4"/>
+      <c r="I13" s="4"/>
+      <c r="J13" s="4"/>
+      <c r="K13" s="4"/>
+      <c r="L13" s="4"/>
+      <c r="M13" s="4"/>
+      <c r="N13" s="4"/>
+    </row>
+    <row r="14" spans="1:14">
       <c r="A14" s="1" t="s">
         <v>21</v>
       </c>
@@ -3677,35 +3674,19 @@
       <c r="E14" s="4">
         <v>44599</v>
       </c>
-      <c r="F14" s="4" t="s">
-        <v>89</v>
-      </c>
-      <c r="G14" s="4" t="s">
-        <v>89</v>
-      </c>
-      <c r="H14" s="4" t="s">
-        <v>89</v>
-      </c>
-      <c r="I14" s="4" t="s">
-        <v>89</v>
-      </c>
-      <c r="J14" s="4" t="s">
-        <v>89</v>
-      </c>
-      <c r="K14" s="4" t="s">
-        <v>89</v>
-      </c>
-      <c r="L14" s="4" t="s">
-        <v>89</v>
-      </c>
-      <c r="M14" s="4" t="s">
-        <v>89</v>
-      </c>
-      <c r="N14" s="4" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="15" spans="1:20">
+      <c r="F14" s="4">
+        <v>44775</v>
+      </c>
+      <c r="G14" s="4"/>
+      <c r="H14" s="4"/>
+      <c r="I14" s="4"/>
+      <c r="J14" s="4"/>
+      <c r="K14" s="4"/>
+      <c r="L14" s="4"/>
+      <c r="M14" s="4"/>
+      <c r="N14" s="4"/>
+    </row>
+    <row r="15" spans="1:14">
       <c r="A15" s="1" t="s">
         <v>23</v>
       </c>
@@ -3721,7 +3702,9 @@
       <c r="E15" s="3">
         <v>1470</v>
       </c>
-      <c r="F15" s="3"/>
+      <c r="F15" s="3">
+        <v>1250</v>
+      </c>
       <c r="G15" s="3"/>
       <c r="H15" s="3"/>
       <c r="I15" s="3"/>
@@ -3730,7 +3713,7 @@
       <c r="L15" s="3"/>
       <c r="M15" s="3"/>
     </row>
-    <row r="16" spans="1:20">
+    <row r="16" spans="1:14">
       <c r="A16" s="1" t="s">
         <v>25</v>
       </c>
@@ -3746,9 +3729,13 @@
       <c r="E16" s="3">
         <v>303.7</v>
       </c>
-      <c r="F16" s="3"/>
+      <c r="F16" s="3">
+        <v>250</v>
+      </c>
       <c r="G16" s="3"/>
-      <c r="H16" s="3"/>
+      <c r="H16" s="3" t="s">
+        <v>89</v>
+      </c>
       <c r="I16" s="3"/>
       <c r="J16" s="3"/>
       <c r="K16" s="3"/>
@@ -3765,13 +3752,15 @@
       <c r="C17" s="3">
         <v>1106</v>
       </c>
-      <c r="D17" s="3">
-        <v>1600</v>
+      <c r="D17" s="19">
+        <v>1066.67</v>
       </c>
       <c r="E17" s="3">
         <v>320.94</v>
       </c>
-      <c r="F17" s="3"/>
+      <c r="F17" s="3">
+        <v>1200</v>
+      </c>
       <c r="G17" s="3"/>
       <c r="H17" s="3"/>
       <c r="I17" s="3"/>
@@ -3809,7 +3798,9 @@
       <c r="E19" s="2">
         <v>1</v>
       </c>
-      <c r="F19" s="2"/>
+      <c r="F19" s="2">
+        <v>1</v>
+      </c>
       <c r="G19" s="2"/>
       <c r="H19" s="2"/>
       <c r="I19" s="2"/>
@@ -3837,7 +3828,9 @@
       <c r="E22" s="2">
         <v>0.5</v>
       </c>
-      <c r="F22" s="2"/>
+      <c r="F22" s="2">
+        <v>0.5</v>
+      </c>
       <c r="G22" s="2"/>
       <c r="H22" s="2"/>
       <c r="I22" s="2"/>
@@ -3869,6 +3862,9 @@
       <c r="E24" s="4">
         <v>44235</v>
       </c>
+      <c r="F24" s="4">
+        <v>44411</v>
+      </c>
     </row>
     <row r="25" spans="1:13">
       <c r="A25" s="1" t="s">
@@ -3881,10 +3877,13 @@
         <v>44561</v>
       </c>
       <c r="D25" s="4">
-        <v>44740</v>
+        <v>44923</v>
       </c>
       <c r="E25" s="4">
         <v>44561</v>
+      </c>
+      <c r="F25" s="4">
+        <v>44594</v>
       </c>
     </row>
     <row r="27" spans="1:13">
@@ -3905,6 +3904,9 @@
       <c r="E28" s="2">
         <v>0.5</v>
       </c>
+      <c r="F28" s="2">
+        <v>0.4</v>
+      </c>
     </row>
     <row r="29" spans="1:13" s="13" customFormat="1">
       <c r="A29" s="1" t="s">
@@ -3927,6 +3929,9 @@
       <c r="E30" s="4">
         <v>44562</v>
       </c>
+      <c r="F30" s="4">
+        <v>44595</v>
+      </c>
     </row>
     <row r="31" spans="1:13">
       <c r="A31" s="1" t="s">
@@ -3941,204 +3946,720 @@
       <c r="E31" s="4">
         <v>44599</v>
       </c>
-    </row>
-    <row r="35" spans="1:5">
-      <c r="B35" s="5" t="s">
+      <c r="F31" s="4">
+        <v>44775</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6">
+      <c r="B33" s="6" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" s="3" customFormat="1">
+      <c r="A34" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="B34" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="C34" s="3">
+        <v>0</v>
+      </c>
+      <c r="D34" s="3">
+        <v>80</v>
+      </c>
+      <c r="E34" s="3">
+        <v>200</v>
+      </c>
+      <c r="F34" s="3">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6">
+      <c r="A35" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="C35" s="4">
+        <v>44231</v>
+      </c>
+      <c r="D35" s="4">
+        <v>44376</v>
+      </c>
+      <c r="E35" s="4">
+        <v>44235</v>
+      </c>
+      <c r="F35" s="4">
+        <v>44348</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6">
+      <c r="A36" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="B36" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="C36" s="4">
+        <v>44595</v>
+      </c>
+      <c r="D36" s="4">
+        <v>44740</v>
+      </c>
+      <c r="E36" s="4">
+        <v>44599</v>
+      </c>
+      <c r="F36" s="4">
+        <v>44561</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6">
+      <c r="B38" s="6" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" s="3" customFormat="1">
+      <c r="A39" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="B39" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="F39" s="3">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6">
+      <c r="A40" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="B40" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="F40" s="4">
+        <v>44562</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6">
+      <c r="A41" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="B41" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="F41" s="4">
+        <v>44843</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6">
+      <c r="B44" s="5" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="37" spans="1:5">
-      <c r="A37" s="1" t="s">
+      <c r="D44" s="3"/>
+    </row>
+    <row r="45" spans="1:6">
+      <c r="C45" s="3"/>
+      <c r="D45" s="3"/>
+    </row>
+    <row r="46" spans="1:6">
+      <c r="A46" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="B37" s="1" t="s">
+      <c r="B46" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="C37" s="1">
+      <c r="C46" s="1">
         <v>2304.17</v>
       </c>
-      <c r="D37" s="1">
+      <c r="D46" s="1">
         <v>2094.89</v>
       </c>
-      <c r="E37" s="1">
+      <c r="E46" s="1">
         <v>1800.45</v>
       </c>
-    </row>
-    <row r="38" spans="1:5">
-      <c r="A38" s="1" t="s">
+      <c r="F46" s="3">
+        <f>F15+F16+F17/12</f>
+        <v>1600</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6">
+      <c r="A47" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="B38" s="1" t="s">
+      <c r="B47" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="C38" s="1">
+      <c r="C47" s="1">
         <v>2304.17</v>
       </c>
-      <c r="D38" s="1">
-        <v>2006</v>
-      </c>
-      <c r="E38" s="1">
+      <c r="D47" s="15">
+        <v>2094.89</v>
+      </c>
+      <c r="E47" s="1">
         <v>1800.45</v>
       </c>
-    </row>
-    <row r="40" spans="1:5">
-      <c r="B40" s="6" t="s">
+      <c r="F47" s="3">
+        <f>F46*F19</f>
+        <v>1600</v>
+      </c>
+    </row>
+    <row r="49" spans="1:16">
+      <c r="B49" s="6" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="50" spans="1:16">
+      <c r="B50" s="8" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="41" spans="1:5">
-      <c r="B41" s="1" t="s">
+      <c r="D50" s="3"/>
+    </row>
+    <row r="51" spans="1:16">
+      <c r="A51" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="B51" s="7" t="s">
         <v>53</v>
       </c>
-      <c r="C41" s="3">
+      <c r="C51" s="3">
         <v>691.25</v>
       </c>
-      <c r="D41" s="3">
+      <c r="D51" s="3">
         <v>628.47</v>
       </c>
-      <c r="E41" s="1">
+      <c r="E51" s="1">
         <v>900.22</v>
       </c>
-    </row>
-    <row r="42" spans="1:5">
-      <c r="A42" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="B42" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="C42" s="1">
+      <c r="F51" s="3">
+        <f>0.5*(F15+F16)+0.5*(F17/12)</f>
+        <v>800</v>
+      </c>
+    </row>
+    <row r="52" spans="1:16" s="3" customFormat="1">
+      <c r="A52" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="B52" s="18" t="s">
+        <v>93</v>
+      </c>
+      <c r="C52" s="3">
         <v>0</v>
       </c>
-      <c r="D42" s="1">
+      <c r="D52" s="3">
         <v>80</v>
       </c>
-      <c r="E42" s="1">
+      <c r="E52" s="3">
         <v>200</v>
       </c>
-    </row>
-    <row r="44" spans="1:5">
-      <c r="B44" s="1" t="s">
+      <c r="F52" s="3">
+        <f>100</f>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="54" spans="1:16">
+      <c r="B54" s="1" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="45" spans="1:5">
-      <c r="A45" s="1" t="s">
+    <row r="55" spans="1:16">
+      <c r="A55" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="B45" s="9" t="s">
+      <c r="B55" s="9" t="s">
         <v>56</v>
       </c>
-      <c r="C45" s="4">
+      <c r="C55" s="4">
         <v>44231</v>
       </c>
-      <c r="D45" s="4">
+      <c r="D55" s="4">
         <v>44376</v>
       </c>
-      <c r="E45" s="4">
+      <c r="E55" s="4">
         <v>44235</v>
       </c>
-    </row>
-    <row r="46" spans="1:5">
-      <c r="A46" s="1" t="s">
+      <c r="F55" s="4">
+        <v>44411</v>
+      </c>
+    </row>
+    <row r="56" spans="1:16">
+      <c r="A56" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="B46" s="9" t="s">
+      <c r="B56" s="9" t="s">
         <v>58</v>
       </c>
-      <c r="C46" s="4">
+      <c r="C56" s="4">
         <v>44595</v>
       </c>
-      <c r="D46" s="4">
+      <c r="D56" s="4">
         <v>44740</v>
       </c>
-      <c r="E46" s="4">
+      <c r="E56" s="4">
         <v>44599</v>
       </c>
-    </row>
-    <row r="47" spans="1:5">
-      <c r="A47" s="1" t="s">
+      <c r="F56" s="4">
+        <v>44561</v>
+      </c>
+    </row>
+    <row r="57" spans="1:16">
+      <c r="A57" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="B47" s="9" t="s">
+      <c r="B57" s="9" t="s">
         <v>60</v>
       </c>
-      <c r="C47" s="11">
-        <f>(DAYS360(C45,C46,TRUE) +1) / 30</f>
+      <c r="C57" s="11">
+        <f>(DAYS360(C55,C56,TRUE) +1) / 30</f>
         <v>12</v>
       </c>
-      <c r="D47" s="11">
-        <f>(DAYS360(D45,D46,TRUE) +1) / 30</f>
+      <c r="D57" s="11">
+        <f>(DAYS360(D55,D56,TRUE) +1) / 30</f>
         <v>12</v>
       </c>
-      <c r="E47" s="1">
+      <c r="E57" s="1">
         <v>12</v>
       </c>
-    </row>
-    <row r="48" spans="1:5">
-      <c r="A48" s="1" t="s">
+      <c r="F57" s="11">
+        <f>(DAYS360(F55,F56,TRUE) +1) / 30</f>
+        <v>4.9333333333333336</v>
+      </c>
+    </row>
+    <row r="58" spans="1:16">
+      <c r="A58" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="B48" s="9" t="s">
+      <c r="B58" s="9" t="s">
         <v>62</v>
       </c>
-      <c r="C48" s="3">
+      <c r="C58" s="3">
         <v>800</v>
       </c>
-      <c r="D48" s="3">
+      <c r="D58" s="3">
         <v>800</v>
       </c>
-      <c r="E48" s="1">
+      <c r="E58" s="1">
         <v>700</v>
       </c>
-    </row>
-    <row r="49" spans="1:5">
-      <c r="A49" s="1" t="s">
+      <c r="F58" s="3">
+        <f>F$47-F51-F52</f>
+        <v>700</v>
+      </c>
+    </row>
+    <row r="59" spans="1:16">
+      <c r="A59" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="B49" s="9" t="s">
+      <c r="B59" s="9" t="s">
         <v>64</v>
       </c>
-      <c r="C49" s="3">
-        <f>C48*C47</f>
+      <c r="C59" s="3">
+        <f>C58*C57</f>
         <v>9600</v>
       </c>
-      <c r="D49" s="3">
-        <f>D48*D47</f>
+      <c r="D59" s="3">
+        <f>D58*D57</f>
         <v>9600</v>
       </c>
-      <c r="E49" s="3">
+      <c r="E59" s="3">
         <v>8400</v>
       </c>
-    </row>
-    <row r="50" spans="1:5">
-      <c r="C50" s="3"/>
-      <c r="D50" s="3"/>
-    </row>
-    <row r="51" spans="1:5">
-      <c r="C51" s="3"/>
-      <c r="D51" s="3"/>
-    </row>
-    <row r="53" spans="1:5">
-      <c r="B53" s="5" t="s">
+      <c r="F59" s="3">
+        <f>F57*F58</f>
+        <v>3453.3333333333335</v>
+      </c>
+    </row>
+    <row r="60" spans="1:16">
+      <c r="C60" s="3"/>
+      <c r="D60" s="3"/>
+    </row>
+    <row r="61" spans="1:16">
+      <c r="B61" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="C61" s="3"/>
+      <c r="D61" s="3"/>
+      <c r="E61" s="3"/>
+    </row>
+    <row r="62" spans="1:16">
+      <c r="C62" s="3"/>
+      <c r="D62" s="3"/>
+      <c r="E62" s="3"/>
+    </row>
+    <row r="63" spans="1:16">
+      <c r="B63" s="8" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="64" spans="1:16">
+      <c r="A64" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="B64" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="C64" s="3"/>
+      <c r="D64" s="3"/>
+      <c r="E64" s="3"/>
+      <c r="F64" s="3">
+        <f>0.5*(F15+F16)+0.5*(F17/12)</f>
+        <v>800</v>
+      </c>
+      <c r="L64" s="1">
+        <v>1617.31</v>
+      </c>
+      <c r="P64" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="65" spans="1:19">
+      <c r="A65" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="B65" s="7" t="s">
+        <v>93</v>
+      </c>
+      <c r="F65" s="1">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="66" spans="1:19">
+      <c r="B66" s="7"/>
+    </row>
+    <row r="67" spans="1:19">
+      <c r="B67" s="7" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="68" spans="1:19">
+      <c r="A68" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="B68" s="9" t="s">
+        <v>56</v>
+      </c>
+      <c r="C68" s="4"/>
+      <c r="D68" s="4"/>
+      <c r="E68" s="4"/>
+      <c r="F68" s="4">
+        <v>44562</v>
+      </c>
+      <c r="L68" s="4">
+        <v>44287</v>
+      </c>
+      <c r="P68" s="4">
+        <v>44615</v>
+      </c>
+      <c r="S68" s="4">
+        <v>44635</v>
+      </c>
+    </row>
+    <row r="69" spans="1:19">
+      <c r="A69" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="B69" s="9" t="s">
+        <v>58</v>
+      </c>
+      <c r="C69" s="4"/>
+      <c r="D69" s="4"/>
+      <c r="E69" s="4"/>
+      <c r="F69" s="4">
+        <v>44594</v>
+      </c>
+      <c r="L69" s="4">
+        <v>44446</v>
+      </c>
+      <c r="P69" s="4">
+        <v>44795</v>
+      </c>
+      <c r="S69" s="4">
+        <v>44818</v>
+      </c>
+    </row>
+    <row r="70" spans="1:19">
+      <c r="A70" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="B70" s="9" t="s">
+        <v>60</v>
+      </c>
+      <c r="C70" s="4"/>
+      <c r="D70" s="4"/>
+      <c r="E70" s="11"/>
+      <c r="F70" s="11">
+        <f>(DAYS360(F68,F69,TRUE) +1) / 30</f>
+        <v>1.0666666666666667</v>
+      </c>
+      <c r="L70" s="1">
+        <v>5.23</v>
+      </c>
+      <c r="P70" s="1">
+        <v>6</v>
+      </c>
+      <c r="S70" s="1">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="71" spans="1:19">
+      <c r="A71" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="B71" s="9" t="s">
+        <v>62</v>
+      </c>
+      <c r="C71" s="3"/>
+      <c r="D71" s="3"/>
+      <c r="E71" s="3"/>
+      <c r="F71" s="3">
+        <f>F$47-F64-F65</f>
+        <v>750</v>
+      </c>
+      <c r="L71" s="1">
+        <v>800</v>
+      </c>
+      <c r="P71" s="1">
+        <v>800</v>
+      </c>
+      <c r="S71" s="1">
+        <v>800</v>
+      </c>
+    </row>
+    <row r="72" spans="1:19">
+      <c r="A72" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="B72" s="9" t="s">
+        <v>64</v>
+      </c>
+      <c r="C72" s="3"/>
+      <c r="D72" s="3"/>
+      <c r="E72" s="3"/>
+      <c r="F72" s="3">
+        <f>F70*F71</f>
+        <v>800</v>
+      </c>
+      <c r="L72" s="1">
+        <v>4187</v>
+      </c>
+      <c r="P72" s="1">
+        <v>4800</v>
+      </c>
+      <c r="S72" s="1">
+        <v>4800</v>
+      </c>
+    </row>
+    <row r="73" spans="1:19">
+      <c r="C73" s="3"/>
+      <c r="D73" s="3"/>
+      <c r="E73" s="3"/>
+    </row>
+    <row r="74" spans="1:19">
+      <c r="B74" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="C74" s="3"/>
+      <c r="D74" s="3"/>
+      <c r="E74" s="3"/>
+    </row>
+    <row r="75" spans="1:19">
+      <c r="C75" s="3"/>
+      <c r="D75" s="3"/>
+      <c r="E75" s="3"/>
+    </row>
+    <row r="76" spans="1:19">
+      <c r="B76" s="8" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="77" spans="1:19">
+      <c r="A77" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="B77" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="C77" s="3"/>
+      <c r="D77" s="3"/>
+      <c r="E77" s="3"/>
+      <c r="F77" s="3">
+        <f>0.4*(F15+F16)+0.4*(F17/12)</f>
+        <v>640</v>
+      </c>
+      <c r="L77" s="1">
+        <v>1617.31</v>
+      </c>
+      <c r="P77" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="78" spans="1:19">
+      <c r="A78" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="B78" s="7" t="s">
+        <v>93</v>
+      </c>
+      <c r="F78" s="1">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="79" spans="1:19">
+      <c r="B79" s="7"/>
+    </row>
+    <row r="80" spans="1:19">
+      <c r="B80" s="7" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="81" spans="1:19">
+      <c r="A81" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="B81" s="9" t="s">
+        <v>56</v>
+      </c>
+      <c r="C81" s="4"/>
+      <c r="D81" s="4"/>
+      <c r="E81" s="4"/>
+      <c r="F81" s="4">
+        <v>44595</v>
+      </c>
+      <c r="L81" s="4">
+        <v>44287</v>
+      </c>
+      <c r="P81" s="4">
+        <v>44615</v>
+      </c>
+      <c r="S81" s="4">
+        <v>44635</v>
+      </c>
+    </row>
+    <row r="82" spans="1:19">
+      <c r="A82" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="B82" s="9" t="s">
+        <v>58</v>
+      </c>
+      <c r="C82" s="4"/>
+      <c r="D82" s="4"/>
+      <c r="E82" s="4"/>
+      <c r="F82" s="4">
+        <v>44775</v>
+      </c>
+      <c r="L82" s="4">
+        <v>44446</v>
+      </c>
+      <c r="P82" s="4">
+        <v>44795</v>
+      </c>
+      <c r="S82" s="4">
+        <v>44818</v>
+      </c>
+    </row>
+    <row r="83" spans="1:19">
+      <c r="A83" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="B83" s="9" t="s">
+        <v>60</v>
+      </c>
+      <c r="C83" s="4"/>
+      <c r="D83" s="4"/>
+      <c r="E83" s="11"/>
+      <c r="F83" s="11">
+        <f>(DAYS360(F81,F82,TRUE) +1) / 30</f>
+        <v>6</v>
+      </c>
+      <c r="L83" s="1">
+        <v>5.23</v>
+      </c>
+      <c r="P83" s="1">
+        <v>6</v>
+      </c>
+      <c r="S83" s="1">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="84" spans="1:19">
+      <c r="A84" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="B84" s="9" t="s">
+        <v>62</v>
+      </c>
+      <c r="C84" s="3"/>
+      <c r="D84" s="3"/>
+      <c r="E84" s="3"/>
+      <c r="F84" s="3">
+        <f>MIN(800, F$47-F77-F78)</f>
+        <v>800</v>
+      </c>
+      <c r="L84" s="1">
+        <v>800</v>
+      </c>
+      <c r="P84" s="1">
+        <v>800</v>
+      </c>
+      <c r="S84" s="1">
+        <v>800</v>
+      </c>
+    </row>
+    <row r="85" spans="1:19">
+      <c r="A85" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="B85" s="9" t="s">
+        <v>64</v>
+      </c>
+      <c r="C85" s="3"/>
+      <c r="D85" s="3"/>
+      <c r="E85" s="3"/>
+      <c r="F85" s="3">
+        <f>F83*F84</f>
+        <v>4800</v>
+      </c>
+      <c r="L85" s="1">
+        <v>4187</v>
+      </c>
+      <c r="P85" s="1">
+        <v>4800</v>
+      </c>
+      <c r="S85" s="1">
+        <v>4800</v>
+      </c>
+    </row>
+    <row r="86" spans="1:19">
+      <c r="C86" s="3"/>
+      <c r="D86" s="3"/>
+      <c r="E86" s="3"/>
+    </row>
+    <row r="87" spans="1:19">
+      <c r="B87" s="5" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="55" spans="1:5">
-      <c r="A55" s="1" t="s">
+    <row r="89" spans="1:19">
+      <c r="A89" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="B55" s="1" t="s">
+      <c r="B89" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="C55" s="3">
+      <c r="C89" s="3">
         <v>9600</v>
       </c>
-      <c r="D55" s="3">
+      <c r="D89" s="3">
         <v>9600</v>
       </c>
-      <c r="E55" s="12">
+      <c r="E89" s="12">
         <v>8400</v>
+      </c>
+      <c r="F89" s="3">
+        <f>ROUND(F85+F72+F59,0)</f>
+        <v>9053</v>
       </c>
     </row>
   </sheetData>
@@ -4153,9 +4674,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -4350,16 +4874,13 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2B13C59C-7030-45E8-A301-EF2965275604}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B745B69C-83B0-4141-8012-52E7AD28B3A0}"/>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -4367,5 +4888,5 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B745B69C-83B0-4141-8012-52E7AD28B3A0}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2B13C59C-7030-45E8-A301-EF2965275604}"/>
 </file>
</xml_diff>